<commit_message>
improve poi files loading
</commit_message>
<xml_diff>
--- a/ZL170517_fish03a_poi.xlsx
+++ b/ZL170517_fish03a_poi.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhikai/Documents/DATA/Ephys/Aerotech_recording_example/20170517/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kagent/Documents/Bagnall lab/DATA/Ephys/Aerotech_recording_example/Processing_codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11080" yWindow="520" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,22 +27,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Filenames</t>
-  </si>
-  <si>
-    <t>Poi1-start</t>
-  </si>
-  <si>
-    <t>Poi1-end</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+  <si>
+    <t>{2:9}</t>
+  </si>
+  <si>
+    <t>{3:10}</t>
+  </si>
+  <si>
+    <t>{5:15}</t>
+  </si>
+  <si>
+    <t>{3:15}</t>
+  </si>
+  <si>
+    <t>{3:7}</t>
+  </si>
+  <si>
+    <t>{2.5:6.5}</t>
+  </si>
+  <si>
+    <t>{1:14}</t>
+  </si>
+  <si>
+    <t>{3:8}</t>
+  </si>
+  <si>
+    <t>{1:9}</t>
+  </si>
+  <si>
+    <t>{1:5}</t>
+  </si>
+  <si>
+    <t>{2:10}</t>
+  </si>
+  <si>
+    <t>{4:11}</t>
+  </si>
+  <si>
+    <t>{2:6}</t>
+  </si>
+  <si>
+    <t>{2:7}</t>
+  </si>
+  <si>
+    <t>{2:5}</t>
+  </si>
+  <si>
+    <t>poi</t>
+  </si>
+  <si>
+    <t>file_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -55,6 +97,29 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -64,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -87,17 +152,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA3A3A3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA3A3A3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,265 +457,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>14</v>
       </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>15</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>16</v>
       </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>17</v>
       </c>
-      <c r="B16" s="1">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>18</v>
       </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>23</v>
       </c>
-      <c r="B18" s="1">
-        <v>2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>24</v>
       </c>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>25</v>
       </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>26</v>
       </c>
-      <c r="B21" s="1">
-        <v>2</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>28</v>
       </c>
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1">
-        <v>5</v>
+      <c r="B23" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>